<commit_message>
Sprint Planning 1.1 version
</commit_message>
<xml_diff>
--- a/Sprint1Planning.xlsx
+++ b/Sprint1Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson\Dropbox\PC\Desktop\DEVELOPPEMENT-APPLICATIOS\projetChantier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F795051F-C95D-4FB5-AB99-E17705A8DBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E3BD9E-3332-4717-91D5-E90057F0D315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{49593094-89CE-44F8-8C8B-C49636785A2F}"/>
   </bookViews>
@@ -544,7 +544,7 @@
   <dimension ref="A1:IH49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4614,9 +4614,10 @@
     </row>
     <row r="25" spans="1:242" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="2">
+      <c r="B25" s="3">
         <v>4</v>
       </c>
+      <c r="C25" s="3"/>
       <c r="I25" t="s">
         <v>12</v>
       </c>
@@ -4852,7 +4853,7 @@
     </row>
     <row r="26" spans="1:242" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>5</v>
       </c>
       <c r="I26" s="2" t="s">
@@ -5086,9 +5087,10 @@
     </row>
     <row r="27" spans="1:242" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="2">
+      <c r="B27" s="3">
         <v>6</v>
       </c>
+      <c r="C27" s="3"/>
       <c r="I27" t="s">
         <v>12</v>
       </c>
@@ -6030,9 +6032,10 @@
     </row>
     <row r="31" spans="1:242" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
-      <c r="B31" s="2">
+      <c r="B31" s="3">
         <v>10</v>
       </c>
+      <c r="C31" s="3"/>
       <c r="I31" t="s">
         <v>12</v>
       </c>
@@ -6268,7 +6271,7 @@
     </row>
     <row r="32" spans="1:242" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
-      <c r="B32">
+      <c r="B32" s="2">
         <v>11</v>
       </c>
       <c r="I32" s="2" t="s">
@@ -6506,9 +6509,10 @@
     </row>
     <row r="33" spans="1:242" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
-      <c r="B33" s="2">
+      <c r="B33" s="3">
         <v>12</v>
       </c>
+      <c r="C33" s="3"/>
       <c r="I33" t="s">
         <v>12</v>
       </c>
@@ -7458,9 +7462,10 @@
     </row>
     <row r="37" spans="1:242" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
-      <c r="B37" s="2">
+      <c r="B37" s="3">
         <v>16</v>
       </c>
+      <c r="C37" s="3"/>
       <c r="I37" t="s">
         <v>12</v>
       </c>
@@ -7696,7 +7701,7 @@
     </row>
     <row r="38" spans="1:242" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
-      <c r="B38">
+      <c r="B38" s="2">
         <v>17</v>
       </c>
       <c r="I38" s="2" t="s">
@@ -7934,9 +7939,10 @@
     </row>
     <row r="39" spans="1:242" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
-      <c r="B39" s="2">
+      <c r="B39" s="3">
         <v>18</v>
       </c>
+      <c r="C39" s="3"/>
       <c r="I39" t="s">
         <v>12</v>
       </c>

</xml_diff>